<commit_message>
perbaiki bug dashboard ojk dan perbamkan
</commit_message>
<xml_diff>
--- a/public/files/contah format import data.xlsx
+++ b/public/files/contah format import data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smurf\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projek\simanis\simanis web baru\simanis_web\public\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{118F235B-56B2-498F-ABA9-C68CF9584714}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{421AD76B-F552-4EDF-80CA-077C6DFF3B98}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{77670124-F1D6-4087-B99A-AEB9F6E89687}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
   <si>
     <t>HAYYUN</t>
   </si>
@@ -99,16 +99,92 @@
   </si>
   <si>
     <t>SADAH</t>
+  </si>
+  <si>
+    <t>NOMOR INDUK KEPENDUDUKAN (NIK)</t>
+  </si>
+  <si>
+    <t>NAMA</t>
+  </si>
+  <si>
+    <t>KAB/KOTA</t>
+  </si>
+  <si>
+    <t>KECAMATAN</t>
+  </si>
+  <si>
+    <t>KELURAHAN/DESA</t>
+  </si>
+  <si>
+    <t>ALAMAT LENGKAP</t>
+  </si>
+  <si>
+    <t>No. Hp</t>
+  </si>
+  <si>
+    <t>Nama Usaha</t>
+  </si>
+  <si>
+    <t>Bentuk Usaha</t>
+  </si>
+  <si>
+    <t>Tahun Berdiri</t>
+  </si>
+  <si>
+    <t>NIB/Tahun</t>
+  </si>
+  <si>
+    <t>Nomor Sertifikat Halal/ Tahun</t>
+  </si>
+  <si>
+    <t>Sertifikat Merek/Tahun</t>
+  </si>
+  <si>
+    <t>Nomor Test Report/Tahun</t>
+  </si>
+  <si>
+    <t>SNI/Tahun</t>
+  </si>
+  <si>
+    <t>Jenis Usaha</t>
+  </si>
+  <si>
+    <t>Cabang Industri</t>
+  </si>
+  <si>
+    <t>Investasi/ Modal (Rp. 000)</t>
+  </si>
+  <si>
+    <t>Jumlah tenaga kerja pria</t>
+  </si>
+  <si>
+    <t>Jumlah tenaga kerja wanita</t>
+  </si>
+  <si>
+    <t>Kapasitas produksi (Rp. 000)</t>
+  </si>
+  <si>
+    <t>Satuan Produksi</t>
+  </si>
+  <si>
+    <t>Nilai produksi (Rp.000)</t>
+  </si>
+  <si>
+    <t>Nilai bahan baku (Rp.000)</t>
+  </si>
+  <si>
+    <t>KBLI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,6 +193,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -156,19 +240,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
+    <cellStyle name="Comma [0] 2" xfId="2" xr:uid="{B938A03A-40B2-402B-9D03-19435DF3F10A}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -481,103 +577,119 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{266EB3F0-D530-483C-A651-68688AF460A3}">
-  <dimension ref="A1:X5"/>
+  <dimension ref="A1:Y6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="11" max="11" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" s="1">
-        <v>211111112</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1">
-        <v>5202</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q1" s="1">
-        <v>3</v>
-      </c>
-      <c r="R1" s="4">
-        <v>15000</v>
-      </c>
-      <c r="S1" s="1">
-        <v>2</v>
-      </c>
-      <c r="T1" s="1">
-        <v>1</v>
-      </c>
-      <c r="U1" s="4">
-        <v>27000</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="W1" s="4">
-        <v>13500</v>
-      </c>
-      <c r="X1" s="4">
-        <v>13500</v>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>211111112</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1">
         <v>5202</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="H2" s="1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>5</v>
@@ -591,39 +703,40 @@
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="Q2" s="1">
+        <v>3</v>
+      </c>
+      <c r="R2" s="4">
+        <v>15000</v>
+      </c>
+      <c r="S2" s="1">
         <v>2</v>
-      </c>
-      <c r="R2" s="4">
-        <v>27000</v>
-      </c>
-      <c r="S2" s="1">
-        <v>5</v>
       </c>
       <c r="T2" s="1">
         <v>1</v>
       </c>
       <c r="U2" s="4">
-        <v>52300</v>
+        <v>27000</v>
       </c>
       <c r="V2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="W2" s="4">
-        <v>26150</v>
+        <v>13500</v>
       </c>
       <c r="X2" s="4">
-        <v>24616</v>
-      </c>
+        <v>13500</v>
+      </c>
+      <c r="Y2" s="8"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>211111113</v>
+        <v>211111112</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1">
         <v>5202</v>
@@ -635,11 +748,11 @@
         <v>10</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="G3" s="3"/>
       <c r="H3" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>5</v>
@@ -653,55 +766,56 @@
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="Q3" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R3" s="4">
-        <v>10000</v>
+        <v>27000</v>
       </c>
       <c r="S3" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="T3" s="1">
         <v>1</v>
       </c>
       <c r="U3" s="4">
-        <v>16000</v>
+        <v>52300</v>
       </c>
       <c r="V3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="W3" s="4">
-        <v>8000</v>
+        <v>26150</v>
       </c>
       <c r="X3" s="4">
-        <v>6000</v>
-      </c>
+        <v>24616</v>
+      </c>
+      <c r="Y3" s="8"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>211111114</v>
+        <v>211111113</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1">
         <v>5202</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>5</v>
@@ -715,39 +829,40 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="Q4" s="1">
         <v>3</v>
       </c>
       <c r="R4" s="4">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="S4" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U4" s="4">
-        <v>1600</v>
+        <v>16000</v>
       </c>
       <c r="V4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="W4" s="4">
-        <v>800</v>
-      </c>
-      <c r="X4" s="1">
-        <v>500</v>
-      </c>
+        <v>8000</v>
+      </c>
+      <c r="X4" s="4">
+        <v>6000</v>
+      </c>
+      <c r="Y4" s="8"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>211111115</v>
+        <v>211111114</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1">
         <v>5202</v>
@@ -756,14 +871,14 @@
         <v>17</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>5</v>
@@ -803,6 +918,70 @@
       <c r="X5" s="1">
         <v>500</v>
       </c>
+      <c r="Y5" s="8"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>211111115</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="1">
+        <v>5202</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J6" s="1">
+        <v>2021</v>
+      </c>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>3</v>
+      </c>
+      <c r="R6" s="4">
+        <v>1000</v>
+      </c>
+      <c r="S6" s="1">
+        <v>2</v>
+      </c>
+      <c r="T6" s="1">
+        <v>2</v>
+      </c>
+      <c r="U6" s="4">
+        <v>1600</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W6" s="4">
+        <v>800</v>
+      </c>
+      <c r="X6" s="1">
+        <v>500</v>
+      </c>
+      <c r="Y6" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix bug imprt badan usaha
</commit_message>
<xml_diff>
--- a/public/files/contah format import data.xlsx
+++ b/public/files/contah format import data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projek\simanis\simanis web baru\simanis_web\public\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data D\simanis\web\simanis_web\public\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{421AD76B-F552-4EDF-80CA-077C6DFF3B98}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8311798-5157-4C01-9A2E-EFE973ADF65C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{77670124-F1D6-4087-B99A-AEB9F6E89687}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{77670124-F1D6-4087-B99A-AEB9F6E89687}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
   <si>
     <t>HAYYUN</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t>KBLI</t>
+  </si>
+  <si>
+    <t>Omset</t>
   </si>
 </sst>
 </file>
@@ -181,8 +184,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -242,22 +245,22 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -577,19 +580,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{266EB3F0-D530-483C-A651-68688AF460A3}">
-  <dimension ref="A1:Y6"/>
+  <dimension ref="A1:Z6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V9" sqref="V9"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="U18" sqref="U18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="11" max="11" width="21.28515625" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="11" max="11" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>23</v>
       </c>
@@ -665,8 +668,11 @@
       <c r="Y1" s="5" t="s">
         <v>47</v>
       </c>
+      <c r="Z1" s="5" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>211111112</v>
       </c>
@@ -730,8 +736,9 @@
         <v>13500</v>
       </c>
       <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>211111112</v>
       </c>
@@ -793,8 +800,9 @@
         <v>24616</v>
       </c>
       <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>211111113</v>
       </c>
@@ -856,8 +864,9 @@
         <v>6000</v>
       </c>
       <c r="Y4" s="8"/>
+      <c r="Z4" s="8"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>211111114</v>
       </c>
@@ -919,8 +928,9 @@
         <v>500</v>
       </c>
       <c r="Y5" s="8"/>
+      <c r="Z5" s="8"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>211111115</v>
       </c>
@@ -982,6 +992,7 @@
         <v>500</v>
       </c>
       <c r="Y6" s="8"/>
+      <c r="Z6" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>